<commit_message>
ES and SHS generated output for CIFMM-2337, CIFMM-2338
</commit_message>
<xml_diff>
--- a/output/EventSummary/immunization-summary-1.xlsx
+++ b/output/EventSummary/immunization-summary-1.xlsx
@@ -14539,7 +14539,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="114" hidden="true">
+    <row r="114">
       <c r="A114" t="s" s="2">
         <v>462</v>
       </c>
@@ -14555,7 +14555,7 @@
         <v>51</v>
       </c>
       <c r="G114" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="H114" t="s" s="2">
         <v>41</v>

</xml_diff>

<commit_message>
Event Summary - regenerate outputs
Eliminated a number of conflict markers left over in some output files
</commit_message>
<xml_diff>
--- a/output/EventSummary/immunization-summary-1.xlsx
+++ b/output/EventSummary/immunization-summary-1.xlsx
@@ -14539,7 +14539,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="114" hidden="true">
+    <row r="114">
       <c r="A114" t="s" s="2">
         <v>462</v>
       </c>
@@ -14555,7 +14555,7 @@
         <v>51</v>
       </c>
       <c r="G114" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="H114" t="s" s="2">
         <v>41</v>

</xml_diff>

<commit_message>
Regenerate outputs for SHS, ES and PHR
There has been some upstream changes in the au-fhir-base, therefore updating our dependent IGs
</commit_message>
<xml_diff>
--- a/output/EventSummary/immunization-summary-1.xlsx
+++ b/output/EventSummary/immunization-summary-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4040" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4040" uniqueCount="449">
   <si>
     <t>Path</t>
   </si>
@@ -725,7 +725,7 @@
     <t>Immunization.manufacturer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org.au/fhir/StructureDefinition/au-organisation]]}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Organization]]}
 </t>
   </si>
   <si>
@@ -1279,10 +1279,6 @@
   </si>
   <si>
     <t>Immunization.vaccinationProtocol.authority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Organization]]}
-</t>
   </si>
   <si>
     <t>Who is responsible for protocol</t>
@@ -3616,7 +3612,7 @@
         <v>41</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="X18" s="2"/>
       <c r="Y18" t="s" s="2">
@@ -12647,13 +12643,13 @@
         <v>41</v>
       </c>
       <c r="J98" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="K98" t="s" s="2">
         <v>406</v>
       </c>
-      <c r="K98" t="s" s="2">
+      <c r="L98" t="s" s="2">
         <v>407</v>
-      </c>
-      <c r="L98" t="s" s="2">
-        <v>408</v>
       </c>
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
@@ -12722,7 +12718,7 @@
         <v>41</v>
       </c>
       <c r="AK98" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AL98" t="s" s="2">
         <v>41</v>
@@ -12736,7 +12732,7 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" t="s" s="2">
@@ -12762,10 +12758,10 @@
         <v>144</v>
       </c>
       <c r="K99" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="L99" t="s" s="2">
         <v>411</v>
-      </c>
-      <c r="L99" t="s" s="2">
-        <v>412</v>
       </c>
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
@@ -12816,7 +12812,7 @@
         <v>41</v>
       </c>
       <c r="AE99" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AF99" t="s" s="2">
         <v>42</v>
@@ -12848,7 +12844,7 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
@@ -12874,10 +12870,10 @@
         <v>397</v>
       </c>
       <c r="K100" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="L100" t="s" s="2">
         <v>414</v>
-      </c>
-      <c r="L100" t="s" s="2">
-        <v>415</v>
       </c>
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
@@ -12928,7 +12924,7 @@
         <v>41</v>
       </c>
       <c r="AE100" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AF100" t="s" s="2">
         <v>42</v>
@@ -12960,7 +12956,7 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -12986,10 +12982,10 @@
         <v>132</v>
       </c>
       <c r="K101" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="L101" t="s" s="2">
         <v>417</v>
-      </c>
-      <c r="L101" t="s" s="2">
-        <v>418</v>
       </c>
       <c r="M101" s="2"/>
       <c r="N101" s="2"/>
@@ -13019,11 +13015,11 @@
         <v>135</v>
       </c>
       <c r="X101" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="Y101" t="s" s="2">
         <v>419</v>
       </c>
-      <c r="Y101" t="s" s="2">
-        <v>420</v>
-      </c>
       <c r="Z101" t="s" s="2">
         <v>41</v>
       </c>
@@ -13040,7 +13036,7 @@
         <v>41</v>
       </c>
       <c r="AE101" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="AF101" t="s" s="2">
         <v>51</v>
@@ -13058,7 +13054,7 @@
         <v>41</v>
       </c>
       <c r="AK101" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AL101" t="s" s="2">
         <v>41</v>
@@ -13072,7 +13068,7 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -13184,7 +13180,7 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
@@ -13298,7 +13294,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -13412,10 +13408,10 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="B105" t="s" s="2">
         <v>424</v>
-      </c>
-      <c r="B105" t="s" s="2">
-        <v>425</v>
       </c>
       <c r="C105" t="s" s="2">
         <v>41</v>
@@ -13440,7 +13436,7 @@
         <v>156</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L105" t="s" s="2">
         <v>158</v>
@@ -13478,7 +13474,7 @@
       </c>
       <c r="X105" s="2"/>
       <c r="Y105" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="Z105" t="s" s="2">
         <v>41</v>
@@ -13528,7 +13524,7 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
@@ -13644,7 +13640,7 @@
     </row>
     <row r="107">
       <c r="A107" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -13670,13 +13666,13 @@
         <v>132</v>
       </c>
       <c r="K107" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="L107" t="s" s="2">
         <v>430</v>
       </c>
-      <c r="L107" t="s" s="2">
+      <c r="M107" t="s" s="2">
         <v>431</v>
-      </c>
-      <c r="M107" t="s" s="2">
-        <v>432</v>
       </c>
       <c r="N107" s="2"/>
       <c r="O107" t="s" s="2">
@@ -13705,46 +13701,46 @@
         <v>135</v>
       </c>
       <c r="X107" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="Y107" t="s" s="2">
         <v>433</v>
       </c>
-      <c r="Y107" t="s" s="2">
+      <c r="Z107" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA107" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB107" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC107" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD107" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE107" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="AF107" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG107" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH107" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI107" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ107" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK107" t="s" s="2">
         <v>434</v>
-      </c>
-      <c r="Z107" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA107" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB107" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC107" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD107" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE107" t="s" s="2">
-        <v>429</v>
-      </c>
-      <c r="AF107" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AG107" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH107" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI107" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ107" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK107" t="s" s="2">
-        <v>435</v>
       </c>
       <c r="AL107" t="s" s="2">
         <v>41</v>
@@ -13758,7 +13754,7 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -13870,7 +13866,7 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
@@ -13984,7 +13980,7 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
@@ -14056,7 +14052,7 @@
         <v>41</v>
       </c>
       <c r="AA110" t="s" s="2">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AB110" s="2"/>
       <c r="AC110" t="s" s="2">
@@ -14098,10 +14094,10 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B111" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C111" t="s" s="2">
         <v>41</v>
@@ -14126,7 +14122,7 @@
         <v>156</v>
       </c>
       <c r="K111" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L111" t="s" s="2">
         <v>158</v>
@@ -14142,7 +14138,7 @@
       </c>
       <c r="P111" s="2"/>
       <c r="Q111" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="R111" t="s" s="2">
         <v>41</v>
@@ -14216,7 +14212,7 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
@@ -14332,7 +14328,7 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
@@ -14358,10 +14354,10 @@
         <v>132</v>
       </c>
       <c r="K113" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="L113" t="s" s="2">
         <v>445</v>
-      </c>
-      <c r="L113" t="s" s="2">
-        <v>446</v>
       </c>
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
@@ -14391,46 +14387,46 @@
         <v>135</v>
       </c>
       <c r="X113" t="s" s="2">
+        <v>446</v>
+      </c>
+      <c r="Y113" t="s" s="2">
         <v>447</v>
       </c>
-      <c r="Y113" t="s" s="2">
+      <c r="Z113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE113" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="AF113" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG113" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK113" t="s" s="2">
         <v>448</v>
-      </c>
-      <c r="Z113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE113" t="s" s="2">
-        <v>444</v>
-      </c>
-      <c r="AF113" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG113" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK113" t="s" s="2">
-        <v>449</v>
       </c>
       <c r="AL113" t="s" s="2">
         <v>41</v>

</xml_diff>

<commit_message>
Regenerate SHS and ES IGs
</commit_message>
<xml_diff>
--- a/output/EventSummary/immunization-summary-1.xlsx
+++ b/output/EventSummary/immunization-summary-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$114</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4040" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4078" uniqueCount="452">
   <si>
     <t>Path</t>
   </si>
@@ -433,7 +433,7 @@
 </t>
   </si>
   <si>
-    <t>Vaccine product administered</t>
+    <t>Vaccine product for administration</t>
   </si>
   <si>
     <t>Vaccine that was administered or was to be administered.</t>
@@ -582,7 +582,7 @@
 </t>
   </si>
   <si>
-    <t>Who was immunized</t>
+    <t>Patient immunised</t>
   </si>
   <si>
     <t>The patient who either received or did not receive the immunization.</t>
@@ -784,7 +784,7 @@
     <t>Immunization.site</t>
   </si>
   <si>
-    <t>Body site vaccine  was administered</t>
+    <t>Body site vaccine was administered</t>
   </si>
   <si>
     <t>Body site where vaccine was administered.</t>
@@ -823,7 +823,7 @@
     <t>Immunization.route</t>
   </si>
   <si>
-    <t>How vaccine entered body</t>
+    <t>Route of vaccination</t>
   </si>
   <si>
     <t>The path by which the vaccine product is taken into the body.</t>
@@ -1054,7 +1054,7 @@
     <t>Immunization.explanation</t>
   </si>
   <si>
-    <t>Administration/non-administration reasons</t>
+    <t>Explanation for (non)vaccination</t>
   </si>
   <si>
     <t>Reasons why a vaccine was or was not administered.</t>
@@ -1072,7 +1072,7 @@
     <t>Immunization.explanation.reason</t>
   </si>
   <si>
-    <t>Why immunization occurred</t>
+    <t>Reason vaccine administered</t>
   </si>
   <si>
     <t>Reasons why a vaccine was administered.</t>
@@ -1229,7 +1229,7 @@
     <t>Immunization.vaccinationProtocol</t>
   </si>
   <si>
-    <t>What protocol was followed</t>
+    <t>Vaccination protocol</t>
   </si>
   <si>
     <t>Contains information about the protocol(s) under which the vaccine was administered.</t>
@@ -1311,7 +1311,7 @@
     <t>Immunization.vaccinationProtocol.targetDisease</t>
   </si>
   <si>
-    <t>Disease immunized against</t>
+    <t>Vaccine disease target</t>
   </si>
   <si>
     <t>The targeted disease.</t>
@@ -1344,13 +1344,26 @@
     <t>https://healthterminologies.gov.au/fhir/ValueSet/vaccination-target-disease-1</t>
   </si>
   <si>
+    <t>targetDiseaseNoInformation</t>
+  </si>
+  <si>
+    <t>No Information for Target Disease</t>
+  </si>
+  <si>
+    <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
+  &lt;system value="http://hl7.org/fhir/v3/NullFlavor"/&gt;
+  &lt;code value="NI"/&gt;
+  &lt;display value="No Information"/&gt;
+&lt;/valueCoding&gt;</t>
+  </si>
+  <si>
     <t>Immunization.vaccinationProtocol.targetDisease.text</t>
   </si>
   <si>
     <t>Immunization.vaccinationProtocol.doseStatus</t>
   </si>
   <si>
-    <t>Indicates if dose counts towards immunity</t>
+    <t>Vaccine relation to protocol</t>
   </si>
   <si>
     <t>Indicates if the immunization event should "count" against  the protocol.</t>
@@ -1561,7 +1574,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO113"/>
+  <dimension ref="A1:AO114"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1571,7 +1584,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="53.76953125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="22.31640625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="26.5390625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -13524,9 +13537,11 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="B106" t="s" s="2">
         <v>427</v>
       </c>
-      <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
         <v>41</v>
       </c>
@@ -13547,26 +13562,26 @@
         <v>52</v>
       </c>
       <c r="J106" t="s" s="2">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="K106" t="s" s="2">
-        <v>172</v>
+        <v>428</v>
       </c>
       <c r="L106" t="s" s="2">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="M106" t="s" s="2">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="N106" t="s" s="2">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="O106" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P106" s="2"/>
       <c r="Q106" t="s" s="2">
-        <v>41</v>
+        <v>429</v>
       </c>
       <c r="R106" t="s" s="2">
         <v>41</v>
@@ -13608,13 +13623,13 @@
         <v>41</v>
       </c>
       <c r="AE106" t="s" s="2">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="AF106" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG106" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH106" t="s" s="2">
         <v>41</v>
@@ -13623,10 +13638,10 @@
         <v>41</v>
       </c>
       <c r="AJ106" t="s" s="2">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="AK106" t="s" s="2">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="AL106" t="s" s="2">
         <v>41</v>
@@ -13638,9 +13653,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -13648,33 +13663,35 @@
       </c>
       <c r="D107" s="2"/>
       <c r="E107" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F107" t="s" s="2">
         <v>51</v>
       </c>
       <c r="G107" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H107" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I107" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H107" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I107" t="s" s="2">
-        <v>41</v>
-      </c>
       <c r="J107" t="s" s="2">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="K107" t="s" s="2">
-        <v>429</v>
+        <v>172</v>
       </c>
       <c r="L107" t="s" s="2">
-        <v>430</v>
+        <v>173</v>
       </c>
       <c r="M107" t="s" s="2">
-        <v>431</v>
-      </c>
-      <c r="N107" s="2"/>
+        <v>174</v>
+      </c>
+      <c r="N107" t="s" s="2">
+        <v>175</v>
+      </c>
       <c r="O107" t="s" s="2">
         <v>41</v>
       </c>
@@ -13698,13 +13715,13 @@
         <v>41</v>
       </c>
       <c r="W107" t="s" s="2">
-        <v>135</v>
+        <v>41</v>
       </c>
       <c r="X107" t="s" s="2">
-        <v>432</v>
+        <v>41</v>
       </c>
       <c r="Y107" t="s" s="2">
-        <v>433</v>
+        <v>41</v>
       </c>
       <c r="Z107" t="s" s="2">
         <v>41</v>
@@ -13722,10 +13739,10 @@
         <v>41</v>
       </c>
       <c r="AE107" t="s" s="2">
-        <v>428</v>
+        <v>176</v>
       </c>
       <c r="AF107" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AG107" t="s" s="2">
         <v>51</v>
@@ -13737,10 +13754,10 @@
         <v>41</v>
       </c>
       <c r="AJ107" t="s" s="2">
-        <v>41</v>
+        <v>177</v>
       </c>
       <c r="AK107" t="s" s="2">
-        <v>434</v>
+        <v>178</v>
       </c>
       <c r="AL107" t="s" s="2">
         <v>41</v>
@@ -13752,9 +13769,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="108" hidden="true">
+    <row r="108">
       <c r="A108" t="s" s="2">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -13762,13 +13779,13 @@
       </c>
       <c r="D108" s="2"/>
       <c r="E108" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F108" t="s" s="2">
         <v>51</v>
       </c>
       <c r="G108" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="H108" t="s" s="2">
         <v>41</v>
@@ -13777,15 +13794,17 @@
         <v>41</v>
       </c>
       <c r="J108" t="s" s="2">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="K108" t="s" s="2">
-        <v>145</v>
+        <v>432</v>
       </c>
       <c r="L108" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="M108" s="2"/>
+        <v>433</v>
+      </c>
+      <c r="M108" t="s" s="2">
+        <v>434</v>
+      </c>
       <c r="N108" s="2"/>
       <c r="O108" t="s" s="2">
         <v>41</v>
@@ -13810,13 +13829,13 @@
         <v>41</v>
       </c>
       <c r="W108" t="s" s="2">
-        <v>41</v>
+        <v>135</v>
       </c>
       <c r="X108" t="s" s="2">
-        <v>41</v>
+        <v>435</v>
       </c>
       <c r="Y108" t="s" s="2">
-        <v>41</v>
+        <v>436</v>
       </c>
       <c r="Z108" t="s" s="2">
         <v>41</v>
@@ -13834,10 +13853,10 @@
         <v>41</v>
       </c>
       <c r="AE108" t="s" s="2">
-        <v>147</v>
+        <v>431</v>
       </c>
       <c r="AF108" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AG108" t="s" s="2">
         <v>51</v>
@@ -13852,7 +13871,7 @@
         <v>41</v>
       </c>
       <c r="AK108" t="s" s="2">
-        <v>148</v>
+        <v>437</v>
       </c>
       <c r="AL108" t="s" s="2">
         <v>41</v>
@@ -13866,18 +13885,18 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="D109" s="2"/>
       <c r="E109" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F109" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G109" t="s" s="2">
         <v>41</v>
@@ -13889,17 +13908,15 @@
         <v>41</v>
       </c>
       <c r="J109" t="s" s="2">
-        <v>97</v>
+        <v>144</v>
       </c>
       <c r="K109" t="s" s="2">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="L109" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="M109" t="s" s="2">
-        <v>100</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="M109" s="2"/>
       <c r="N109" s="2"/>
       <c r="O109" t="s" s="2">
         <v>41</v>
@@ -13936,25 +13953,25 @@
         <v>41</v>
       </c>
       <c r="AA109" t="s" s="2">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="AB109" t="s" s="2">
-        <v>152</v>
+        <v>41</v>
       </c>
       <c r="AC109" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD109" t="s" s="2">
-        <v>153</v>
+        <v>41</v>
       </c>
       <c r="AE109" t="s" s="2">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="AF109" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG109" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH109" t="s" s="2">
         <v>41</v>
@@ -13980,11 +13997,11 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="D110" s="2"/>
       <c r="E110" t="s" s="2">
@@ -14000,23 +14017,21 @@
         <v>41</v>
       </c>
       <c r="I110" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="J110" t="s" s="2">
-        <v>156</v>
+        <v>97</v>
       </c>
       <c r="K110" t="s" s="2">
-        <v>157</v>
+        <v>98</v>
       </c>
       <c r="L110" t="s" s="2">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="M110" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="N110" t="s" s="2">
-        <v>160</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="N110" s="2"/>
       <c r="O110" t="s" s="2">
         <v>41</v>
       </c>
@@ -14052,9 +14067,11 @@
         <v>41</v>
       </c>
       <c r="AA110" t="s" s="2">
-        <v>438</v>
-      </c>
-      <c r="AB110" s="2"/>
+        <v>151</v>
+      </c>
+      <c r="AB110" t="s" s="2">
+        <v>152</v>
+      </c>
       <c r="AC110" t="s" s="2">
         <v>41</v>
       </c>
@@ -14062,7 +14079,7 @@
         <v>153</v>
       </c>
       <c r="AE110" t="s" s="2">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="AF110" t="s" s="2">
         <v>42</v>
@@ -14077,10 +14094,10 @@
         <v>41</v>
       </c>
       <c r="AJ110" t="s" s="2">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="AK110" t="s" s="2">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="AL110" t="s" s="2">
         <v>41</v>
@@ -14094,11 +14111,9 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>437</v>
-      </c>
-      <c r="B111" t="s" s="2">
-        <v>439</v>
-      </c>
+        <v>440</v>
+      </c>
+      <c r="B111" s="2"/>
       <c r="C111" t="s" s="2">
         <v>41</v>
       </c>
@@ -14107,7 +14122,7 @@
         <v>42</v>
       </c>
       <c r="F111" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G111" t="s" s="2">
         <v>41</v>
@@ -14122,7 +14137,7 @@
         <v>156</v>
       </c>
       <c r="K111" t="s" s="2">
-        <v>440</v>
+        <v>157</v>
       </c>
       <c r="L111" t="s" s="2">
         <v>158</v>
@@ -14138,46 +14153,44 @@
       </c>
       <c r="P111" s="2"/>
       <c r="Q111" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R111" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S111" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T111" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U111" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V111" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W111" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X111" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y111" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z111" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA111" t="s" s="2">
         <v>441</v>
       </c>
-      <c r="R111" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S111" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T111" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U111" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V111" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W111" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X111" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y111" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z111" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA111" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB111" t="s" s="2">
-        <v>41</v>
-      </c>
+      <c r="AB111" s="2"/>
       <c r="AC111" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD111" t="s" s="2">
-        <v>41</v>
+        <v>153</v>
       </c>
       <c r="AE111" t="s" s="2">
         <v>162</v>
@@ -14212,9 +14225,11 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="B112" t="s" s="2">
         <v>442</v>
       </c>
-      <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
         <v>41</v>
       </c>
@@ -14235,26 +14250,26 @@
         <v>52</v>
       </c>
       <c r="J112" t="s" s="2">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>172</v>
+        <v>443</v>
       </c>
       <c r="L112" t="s" s="2">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="M112" t="s" s="2">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="N112" t="s" s="2">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="O112" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P112" s="2"/>
       <c r="Q112" t="s" s="2">
-        <v>41</v>
+        <v>444</v>
       </c>
       <c r="R112" t="s" s="2">
         <v>41</v>
@@ -14296,13 +14311,13 @@
         <v>41</v>
       </c>
       <c r="AE112" t="s" s="2">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="AF112" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG112" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH112" t="s" s="2">
         <v>41</v>
@@ -14311,10 +14326,10 @@
         <v>41</v>
       </c>
       <c r="AJ112" t="s" s="2">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="AK112" t="s" s="2">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="AL112" t="s" s="2">
         <v>41</v>
@@ -14328,7 +14343,7 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
@@ -14348,19 +14363,23 @@
         <v>41</v>
       </c>
       <c r="I113" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="J113" t="s" s="2">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="K113" t="s" s="2">
-        <v>444</v>
+        <v>172</v>
       </c>
       <c r="L113" t="s" s="2">
-        <v>445</v>
-      </c>
-      <c r="M113" s="2"/>
-      <c r="N113" s="2"/>
+        <v>173</v>
+      </c>
+      <c r="M113" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="N113" t="s" s="2">
+        <v>175</v>
+      </c>
       <c r="O113" t="s" s="2">
         <v>41</v>
       </c>
@@ -14384,62 +14403,174 @@
         <v>41</v>
       </c>
       <c r="W113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE113" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="AF113" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG113" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ113" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="AK113" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="AL113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AM113" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN113" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="114" hidden="true">
+      <c r="A114" t="s" s="2">
+        <v>446</v>
+      </c>
+      <c r="B114" s="2"/>
+      <c r="C114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D114" s="2"/>
+      <c r="E114" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F114" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J114" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="K114" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="L114" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="M114" s="2"/>
+      <c r="N114" s="2"/>
+      <c r="O114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P114" s="2"/>
+      <c r="Q114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W114" t="s" s="2">
         <v>135</v>
       </c>
-      <c r="X113" t="s" s="2">
+      <c r="X114" t="s" s="2">
+        <v>449</v>
+      </c>
+      <c r="Y114" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="Z114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE114" t="s" s="2">
         <v>446</v>
       </c>
-      <c r="Y113" t="s" s="2">
-        <v>447</v>
-      </c>
-      <c r="Z113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE113" t="s" s="2">
-        <v>443</v>
-      </c>
-      <c r="AF113" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG113" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK113" t="s" s="2">
-        <v>448</v>
-      </c>
-      <c r="AL113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AM113" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AN113" t="s" s="2">
+      <c r="AF114" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG114" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK114" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="AL114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AM114" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN114" t="s" s="2">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN113">
+  <autoFilter ref="A1:AN114">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -14449,7 +14580,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI112">
+  <conditionalFormatting sqref="A2:AI113">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>